<commit_message>
NB Reporting: 1)kzt form 8 - removed empty records 2)kzt form 13 - added export template formatting (numbers with decimals)
</commit_message>
<xml_diff>
--- a/nicnbk-data/nicnbk-data-service-impl/src/main/resources/export_template/reporting/TEMPLATE_NICKMF_cons_KZT_13.xlsx
+++ b/nicnbk-data/nicnbk-data-service-impl/src/main/resources/export_template/reporting/TEMPLATE_NICKMF_cons_KZT_13.xlsx
@@ -347,7 +347,7 @@
     <xf numFmtId="164" fontId="1" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="48">
+  <cellXfs count="49">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
@@ -474,6 +474,9 @@
     </xf>
     <xf numFmtId="0" fontId="10" fillId="0" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="4" fontId="10" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="top"/>
     </xf>
   </cellXfs>
   <cellStyles count="3">
@@ -796,8 +799,8 @@
   </sheetPr>
   <dimension ref="A1:AL56"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A4" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="A16" sqref="A16:XFD16"/>
+    <sheetView tabSelected="1" topLeftCell="G10" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="K16" sqref="K16"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1378,29 +1381,29 @@
       <c r="G16" s="39"/>
       <c r="H16" s="36"/>
       <c r="I16" s="36"/>
-      <c r="J16" s="36"/>
-      <c r="K16" s="36"/>
-      <c r="L16" s="36"/>
-      <c r="M16" s="36"/>
-      <c r="N16" s="36"/>
-      <c r="O16" s="36"/>
-      <c r="P16" s="36"/>
-      <c r="Q16" s="36"/>
-      <c r="R16" s="36"/>
-      <c r="S16" s="36"/>
-      <c r="T16" s="36"/>
-      <c r="U16" s="36"/>
-      <c r="V16" s="36"/>
-      <c r="W16" s="36"/>
-      <c r="X16" s="36"/>
-      <c r="Y16" s="36"/>
-      <c r="Z16" s="36"/>
-      <c r="AA16" s="36"/>
-      <c r="AB16" s="36"/>
-      <c r="AC16" s="36"/>
-      <c r="AD16" s="36"/>
-      <c r="AE16" s="36"/>
-      <c r="AF16" s="36"/>
+      <c r="J16" s="48"/>
+      <c r="K16" s="48"/>
+      <c r="L16" s="48"/>
+      <c r="M16" s="48"/>
+      <c r="N16" s="48"/>
+      <c r="O16" s="48"/>
+      <c r="P16" s="48"/>
+      <c r="Q16" s="48"/>
+      <c r="R16" s="48"/>
+      <c r="S16" s="48"/>
+      <c r="T16" s="48"/>
+      <c r="U16" s="48"/>
+      <c r="V16" s="48"/>
+      <c r="W16" s="48"/>
+      <c r="X16" s="48"/>
+      <c r="Y16" s="48"/>
+      <c r="Z16" s="48"/>
+      <c r="AA16" s="48"/>
+      <c r="AB16" s="48"/>
+      <c r="AC16" s="48"/>
+      <c r="AD16" s="48"/>
+      <c r="AE16" s="48"/>
+      <c r="AF16" s="48"/>
       <c r="AG16" s="17"/>
     </row>
     <row r="17" spans="1:38" x14ac:dyDescent="0.25">

</xml_diff>